<commit_message>
update the project task
</commit_message>
<xml_diff>
--- a/项目发展记录.xlsx
+++ b/项目发展记录.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hub\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wps_deco_share\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="关键决策点记录" sheetId="1" r:id="rId1"/>
-    <sheet name="站点内容策划" sheetId="2" r:id="rId2"/>
+    <sheet name="站点运营" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>分类序号</t>
   </si>
@@ -129,13 +129,94 @@
 这样做的好处是在潜移默化中选择我们的客户和极匠。
 比如：我们可以宣传我们开放式装修的理念，说明它和全包、清包之间的不同。让用户理解这样做的好处，理解我们的服务理念。
 比如：我们对极匠可以宣传我们新的工作理念，说明它相比坐班制的优越性，相比工作室的优越性。</t>
+  </si>
+  <si>
+    <t>类型</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>内容类：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>主要是指站点上放置内容的一些想法和策划。站点的内容直接影响着用户对站点的认识，没有经过考虑直接添加往往会导致问题。</t>
+    </r>
+  </si>
+  <si>
+    <t>通过打通物业，让物业工作为极匠空间的服务提供宣传。</t>
+  </si>
+  <si>
+    <t>内容类</t>
+  </si>
+  <si>
+    <t>陆璜</t>
+  </si>
+  <si>
+    <t>渠道类</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>渠道类：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>指有哪些渠道可以用于拓展市场活动。</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>市场类：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>指市场活动可以通过何种形式，或者何种方式展开的一些策划和考虑。</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,6 +229,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -512,7 +600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
@@ -799,20 +887,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="115.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.42578125" customWidth="1"/>
+    <col min="3" max="4" width="17.5703125" customWidth="1"/>
+    <col min="5" max="5" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -823,10 +911,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -836,11 +927,50 @@
       <c r="C2" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="6">
         <v>42895</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="6">
+        <v>42898</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>